<commit_message>
Before deleting all old folders for background
</commit_message>
<xml_diff>
--- a/backgrounds/Attributes.xlsx
+++ b/backgrounds/Attributes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Acolyte</t>
   </si>
@@ -44,13 +44,109 @@
   </si>
   <si>
     <t>City Watch</t>
+  </si>
+  <si>
+    <t>Insight=Religion</t>
+  </si>
+  <si>
+    <t>History=Survival</t>
+  </si>
+  <si>
+    <t>Acrobatics=Athletics</t>
+  </si>
+  <si>
+    <t>Insight=Intimidation</t>
+  </si>
+  <si>
+    <t>Deception=Insight</t>
+  </si>
+  <si>
+    <t>Athletics=Intimidation</t>
+  </si>
+  <si>
+    <t>Animal Handling=Survival</t>
+  </si>
+  <si>
+    <t>Perception=Performance</t>
+  </si>
+  <si>
+    <t>Deception=Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Athletics=Insight</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Navigator’s tools</t>
+  </si>
+  <si>
+    <t>Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Disguise Kit=One Type of Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>One Type of Gaming Set</t>
+  </si>
+  <si>
+    <t>Land Vehicles</t>
+  </si>
+  <si>
+    <t>Disguise Kit</t>
+  </si>
+  <si>
+    <t>Disguise Kit=Forgery Kit</t>
+  </si>
+  <si>
+    <t>Any=Any</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Celestial=Draconic</t>
+  </si>
+  <si>
+    <t>A Holy Symbol=A Prayer Book=5 Sticks of Incense=Vestments=a Set of Common Clothes=A Belt Pouch which is Containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Leather-Bound Diary=A Bottle of Ink=An Ink Pen=A Set of Traveler’s Clothes=One Trinket of Special Significance=A Pouch Containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Wooden Case Containing a Map to a Ruin=A Bullseye Lantern=A Miner’s Pick=A Set of Traveler’s Clothes=A Shovel=A Two-Person Tent=A Trinket Recovered from a Dig Site=A Pouch Containing 25 gp</t>
+  </si>
+  <si>
+    <t>A Leather Ball=A Lucky Charm=A Set of Traveler’s Clothes=A Pouch Containing 10 gp</t>
+  </si>
+  <si>
+    <t>An Azorius Insignia=A Scroll Containing the Text of a Law Important to you=A Bottle of Blue Ink=A Pen=A Set of Fine Clothes=A Belt Pouch Containing 10 gp (Azorius-minted 1-zino coins)</t>
+  </si>
+  <si>
+    <t>Disguise Kit=Common Clothes=A Tears of Virulence Emblem=A Writ of Free Agency Signed by the Lord Regent=A Set of Artisan’s Tools you are Proficient With=A Pouch with 15 gp (payment for services rendered)</t>
+  </si>
+  <si>
+    <t>A Boros Insignia=A Feather from an Angel’s Wing=A Tattered Piece of a Boros Banner (A Souvenir from a Famous Battle)=A Set of Common Clothes=A Belt Pouch Containing 2gp (Boros-minted 1-zino coins)</t>
+  </si>
+  <si>
+    <t>A Whip=A Tent=A Regional Map=A Set of Traveling Clothes=Belt Pouch Containing 10 gp</t>
+  </si>
+  <si>
+    <t>Disguise kit=A Set of Fine Clothes=Belt Pouch Containing 30 gp(gold piece)</t>
+  </si>
+  <si>
+    <t>A Set of Fine Clothes=Disguise Kit=Tools of the Con of your Choice (Ten Stoppered Bottles filled with Colored Liquid, a Set of Weighted Dice, a Deck of Marked Cards, or a Signet Ring of an Imaginary Duke)=Belt Pouch Containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Uniform in the Style of your Unit=Indicative of your Rank=Horn with which to Summon Help=A Set of Manacles=A Pouch Containing 10 gp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -60,6 +156,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,12 +177,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -334,6 +438,146 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Beginning work on dndclass
</commit_message>
<xml_diff>
--- a/backgrounds/Attributes.xlsx
+++ b/backgrounds/Attributes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="158">
   <si>
     <t>Acolyte</t>
   </si>
@@ -46,6 +46,105 @@
     <t>City Watch</t>
   </si>
   <si>
+    <t>Clan Crafter</t>
+  </si>
+  <si>
+    <t>Cloistered Scholar</t>
+  </si>
+  <si>
+    <t>Cormanthor Refugee</t>
+  </si>
+  <si>
+    <t>Courtier</t>
+  </si>
+  <si>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>Dragon Casualty</t>
+  </si>
+  <si>
+    <t>Earthspur Miner</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>Failed Merchant</t>
+  </si>
+  <si>
+    <t>Faceless</t>
+  </si>
+  <si>
+    <t>Entertainer</t>
+  </si>
+  <si>
+    <t>Far Traveler</t>
+  </si>
+  <si>
+    <t>Folk Hero</t>
+  </si>
+  <si>
+    <t>Gate Urchin</t>
+  </si>
+  <si>
+    <t>Golgari Agent</t>
+  </si>
+  <si>
+    <t>Gruul Anarch</t>
+  </si>
+  <si>
+    <t>Gambler</t>
+  </si>
+  <si>
+    <t>Guild Merchant</t>
+  </si>
+  <si>
+    <t>Guild Artisan</t>
+  </si>
+  <si>
+    <t>Harborfolk</t>
+  </si>
+  <si>
+    <t>Haunted One</t>
+  </si>
+  <si>
+    <t>Hermit</t>
+  </si>
+  <si>
+    <t>Hillsfar Merchant</t>
+  </si>
+  <si>
+    <t>Hillsfar Smuggler</t>
+  </si>
+  <si>
+    <t>House Agent</t>
+  </si>
+  <si>
+    <t>Inheritor</t>
+  </si>
+  <si>
+    <t>Initiate</t>
+  </si>
+  <si>
+    <t>Inquisitor</t>
+  </si>
+  <si>
+    <t>Iron Route Bandit</t>
+  </si>
+  <si>
+    <t>Izzet Engineer</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Smuggler</t>
+  </si>
+  <si>
+    <t>Spy</t>
+  </si>
+  <si>
     <t>Insight=Religion</t>
   </si>
   <si>
@@ -76,6 +175,72 @@
     <t>Athletics=Insight</t>
   </si>
   <si>
+    <t>History=Insight</t>
+  </si>
+  <si>
+    <t>History=Arcana</t>
+  </si>
+  <si>
+    <t>Nature=Survival</t>
+  </si>
+  <si>
+    <t>Insight=Persuasion</t>
+  </si>
+  <si>
+    <t>Deception=Stealth</t>
+  </si>
+  <si>
+    <t>Intimidation=Survival</t>
+  </si>
+  <si>
+    <t>Athletics=Survival</t>
+  </si>
+  <si>
+    <t>Investigation=Persuation</t>
+  </si>
+  <si>
+    <t>Deception=Intimidation</t>
+  </si>
+  <si>
+    <t>Acrobatics=Performance</t>
+  </si>
+  <si>
+    <t>Insight=Perception</t>
+  </si>
+  <si>
+    <t>Animal Handling=Athletics</t>
+  </si>
+  <si>
+    <t>Athletics=Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Arcana=Investigation</t>
+  </si>
+  <si>
+    <t>Medicine=Religion</t>
+  </si>
+  <si>
+    <t>Perception=Stealth</t>
+  </si>
+  <si>
+    <t>Investigation=Persuasion</t>
+  </si>
+  <si>
+    <t>Survival=History</t>
+  </si>
+  <si>
+    <t>Investigation=Religion</t>
+  </si>
+  <si>
+    <t>Stealth=Animal Handling</t>
+  </si>
+  <si>
+    <t>History=Persuasion</t>
+  </si>
+  <si>
+    <t>Athletics=Deception</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
@@ -100,6 +265,66 @@
     <t>Disguise Kit=Forgery Kit</t>
   </si>
   <si>
+    <t>One Type of Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>One type of Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>One Type of Gaming Set=Thieves’ Tools</t>
+  </si>
+  <si>
+    <t>Vehicles (water)</t>
+  </si>
+  <si>
+    <t>Disguise Kit=One Type of Musical Instrument</t>
+  </si>
+  <si>
+    <t>One Musical Instrument</t>
+  </si>
+  <si>
+    <t>One Type of Artisan’s Tools=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Thieves’ tools=One Type of Musical Instrument</t>
+  </si>
+  <si>
+    <t>Tool Proficiencies: Poisoner’s kit</t>
+  </si>
+  <si>
+    <t>Herbalism Kit</t>
+  </si>
+  <si>
+    <t>One gaming set</t>
+  </si>
+  <si>
+    <t>Navigator’s Tools</t>
+  </si>
+  <si>
+    <t>One Type of Gaming Set=Vehicles (Water)</t>
+  </si>
+  <si>
+    <t>Herbalism kit</t>
+  </si>
+  <si>
+    <t>Vehicles (Land)=Vehicles (Water)</t>
+  </si>
+  <si>
+    <t>Forgery kit</t>
+  </si>
+  <si>
+    <t>A Musical Instrument</t>
+  </si>
+  <si>
+    <t>One Type of Gaming Set=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Thieves’ Tools=One Set of Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>Vehicles (Water)</t>
+  </si>
+  <si>
     <t>Any=Any</t>
   </si>
   <si>
@@ -109,6 +334,27 @@
     <t>Celestial=Draconic</t>
   </si>
   <si>
+    <t>Dwarvish</t>
+  </si>
+  <si>
+    <t>Elven</t>
+  </si>
+  <si>
+    <t>Draconic</t>
+  </si>
+  <si>
+    <t>Dwarven=Undercommon</t>
+  </si>
+  <si>
+    <t>Elvish</t>
+  </si>
+  <si>
+    <t>Abyssal</t>
+  </si>
+  <si>
+    <t>Vedalken</t>
+  </si>
+  <si>
     <t>A Holy Symbol=A Prayer Book=5 Sticks of Incense=Vestments=a Set of Common Clothes=A Belt Pouch which is Containing 15 gp</t>
   </si>
   <si>
@@ -140,6 +386,105 @@
   </si>
   <si>
     <t>A Uniform in the Style of your Unit=Indicative of your Rank=Horn with which to Summon Help=A Set of Manacles=A Pouch Containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Set of Artisan’s Tools with which you are proficient=A Maker’s Mark Chisel used to mark your Handiwork with the Symbol of the Clan of Crafters you learned your Skill from=A Set of Traveler’s Clothes=A Pouch containing 5 gp=A Gem worth 10 gp</t>
+  </si>
+  <si>
+    <t>The Scholar’s Robes of your Cloister=A Writing Kit (Small Pouch with a Quill, Ink, Folded Parchment, and a Small Penknife)=A Borrowed Book on the Subject of your Current Study=A Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Two-Person Tent=Artisan’s Tools=A Holy Symbol=A Set of Traveler’s Clothes=A Belt Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>A Set of Fine Clothes=A Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>A Crowbar=A Set of Dark Common Clothes including a Hood=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Dagger=Tattered Rags=A Loaf of Moldy Bread=A Small Cast-Off Scale belonging to Vorgansharax – the Maimed Virulence=A Pouch with 5 gp of Various Coins (salvaged during your escape from Phlan)</t>
+  </si>
+  <si>
+    <t>A Shovel=A Block and Tackle=A Climber’s Kit=A Set of Common Clothes=A Belt Pouch containing 5 gp.</t>
+  </si>
+  <si>
+    <t>Fishing tackle=A Net=A Favorite Fishing Lure=A Set of Traveler’s Clothes=A Belt Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>One Set of Artisan’s Tools=Merchant’s Scale=A Set of Fine Clothes=A Belt Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A disguise Kit=A Costume=A Pouch containing 10gp</t>
+  </si>
+  <si>
+    <t>One Musical Instrument=The Favor of an Admirer (Trinket)=A Costume=A Belt Pouch containing 15 gp.</t>
+  </si>
+  <si>
+    <t>One Set of Traveler’s Clothes=One Musical Instrument=Poorly Wrought Maps from your Homeland that Depict where you are in Faerûn=A Small Piece of Jewelry worth 10 gp in the Style of your Homeland’s Craftsmanship=A Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>A Set of Artisan’s Tools=A Shovel=An Iron Pot=A Set of Common Clothes=A Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Battered Alms Box=A Musical Instrument=A Cast-Off Military Jacket=A Set of Common Clothes=A Belt Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Golgari Insignia=A Poisoner’s Kit=A Pet Beetle=A Set of Common Clothes=A Belt Pouch containing 10 gp worth of Mixed Coins</t>
+  </si>
+  <si>
+    <t>A Gruul Insignia=A Hunting Trap=An Herbalism Kit=The Skull of a Boar=A Beast-Hide Cloak=A Set of Traveler’s Clothes=A Pouch containing 10gp (Azorius 1-zino coins)</t>
+  </si>
+  <si>
+    <t>One Gaming Set=A Lucky Charm=A Set of Fine Clothes=A Belt Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Mule=A Cart=A Letter of Introduction from your Guild=A Set of Traveler’s Clothes=A Belt Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Set of Artisan’s Tools=A Letter of Introduction from your Guild=A Set of Traveler’s Clothes=A Belt Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>Fishing tackle=Dice Set=A Set of Common Clothes=Rowboat=A Belt containing 5 gp</t>
+  </si>
+  <si>
+    <t>Monster Hunter’s Pack=One Trinket of Special Significance</t>
+  </si>
+  <si>
+    <t>A Scroll Case stuffed Full of Notes from your Studies=A Winter Blanket=A Set of Common Clothes=An Herbalism Kit=5 gp</t>
+  </si>
+  <si>
+    <t>A Fine Set of Clothes=A Signet Ring=A Letter of Introduction from your Family’s Trading House=A Purse containing 25 gp</t>
+  </si>
+  <si>
+    <t>A Forgery Kit=A Set of Common Clothes=A Belt Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>A Set of Fine Clothes=House Signet Ring=Identification Papers=A Purse containing 20 gp</t>
+  </si>
+  <si>
+    <t>Your Inheritance=A Set of Traveler’s Clothes=A Musical Instrument=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Simple Puzzle Box=A Scroll containing the Basic Teachings of the Five Gods=A Gaming Set=A Set of Common Clothes=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Holy Symbol=A Set of Traveler’s Clothes=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Set of Dark Common Clothes=Pack Saddle=Burglar’s Pack=A Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>An Izzet Insignia=One Set of Artisan’s Tools=The Charred and Twisted remains of a Failed Experiment=A Hammer=A Block and Tackle=A Set of Common Clothes=A Belt Pouch containing 5 gp (Azorius 1-Zino Coins)</t>
+  </si>
+  <si>
+    <t>A Set of Fine Clothes=A Signet Ring=A Scroll of Pedigree=A Purse containing 25 gp</t>
+  </si>
+  <si>
+    <t>A Fancy Leather Vest=A Set of Common Clothes=A Leather Pouch with 15 gp</t>
+  </si>
+  <si>
+    <t>A crowbar=A Set of Dark Common Clothes including a Hood=A Pouch containing 15 gp</t>
   </si>
 </sst>
 </file>
@@ -437,145 +782,640 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>53</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>29</v>
+        <v>104</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>42</v>
+        <v>124</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Class archetypes added, along with tool types
</commit_message>
<xml_diff>
--- a/backgrounds/Attributes.xlsx
+++ b/backgrounds/Attributes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
   <si>
     <t>Acolyte</t>
   </si>
@@ -250,13 +250,10 @@
     <t>Vehicles (Land)</t>
   </si>
   <si>
-    <t>Disguise Kit=One Type of Artisan’s Tools</t>
-  </si>
-  <si>
-    <t>One Type of Gaming Set</t>
-  </si>
-  <si>
-    <t>Land Vehicles</t>
+    <t>Disguise Kit=*Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>*Gaming Sets</t>
   </si>
   <si>
     <t>Disguise Kit</t>
@@ -265,43 +262,37 @@
     <t>Disguise Kit=Forgery Kit</t>
   </si>
   <si>
-    <t>One Type of Artisan’s Tools</t>
-  </si>
-  <si>
-    <t>One type of Artisan’s Tools</t>
-  </si>
-  <si>
-    <t>One Type of Gaming Set=Thieves’ Tools</t>
-  </si>
-  <si>
-    <t>Vehicles (water)</t>
-  </si>
-  <si>
-    <t>Disguise Kit=One Type of Musical Instrument</t>
-  </si>
-  <si>
-    <t>One Musical Instrument</t>
-  </si>
-  <si>
-    <t>One Type of Artisan’s Tools=Vehicles (Land)</t>
-  </si>
-  <si>
-    <t>Thieves’ tools=One Type of Musical Instrument</t>
-  </si>
-  <si>
-    <t>Tool Proficiencies: Poisoner’s kit</t>
+    <t>*Artisan’s Tools</t>
+  </si>
+  <si>
+    <t>*Gaming Sets=Thieves’ Tools</t>
+  </si>
+  <si>
+    <t>Vehicles (Water)</t>
+  </si>
+  <si>
+    <t>Disguise Kit=*Musical Instruments</t>
+  </si>
+  <si>
+    <t>*Musical Instruments</t>
+  </si>
+  <si>
+    <t>*Artisan’s Tools=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Thieves’ tools=*Musical Instruments</t>
+  </si>
+  <si>
+    <t>Poisoner’s kit</t>
   </si>
   <si>
     <t>Herbalism Kit</t>
   </si>
   <si>
-    <t>One gaming set</t>
-  </si>
-  <si>
     <t>Navigator’s Tools</t>
   </si>
   <si>
-    <t>One Type of Gaming Set=Vehicles (Water)</t>
+    <t>*Gaming Sets=Vehicles (Water)</t>
   </si>
   <si>
     <t>Herbalism kit</t>
@@ -313,16 +304,10 @@
     <t>Forgery kit</t>
   </si>
   <si>
-    <t>A Musical Instrument</t>
-  </si>
-  <si>
-    <t>One Type of Gaming Set=Vehicles (Land)</t>
-  </si>
-  <si>
-    <t>Thieves’ Tools=One Set of Artisan’s Tools</t>
-  </si>
-  <si>
-    <t>Vehicles (Water)</t>
+    <t>*Gaming Sets=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>Thieves’ Tools=*Artisan’s Tools</t>
   </si>
   <si>
     <t>Any=Any</t>
@@ -370,7 +355,7 @@
     <t>An Azorius Insignia=A Scroll Containing the Text of a Law Important to you=A Bottle of Blue Ink=A Pen=A Set of Fine Clothes=A Belt Pouch Containing 10 gp (Azorius-minted 1-zino coins)</t>
   </si>
   <si>
-    <t>Disguise Kit=Common Clothes=A Tears of Virulence Emblem=A Writ of Free Agency Signed by the Lord Regent=A Set of Artisan’s Tools you are Proficient With=A Pouch with 15 gp (payment for services rendered)</t>
+    <t>Disguise Kit=Common Clothes=A Tears of Virulence Emblem=A Writ of Free Agency Signed by the Lord Regent=*Artisan’s Tools=A Pouch with 15 gp (payment for services rendered)</t>
   </si>
   <si>
     <t>A Boros Insignia=A Feather from an Angel’s Wing=A Tattered Piece of a Boros Banner (A Souvenir from a Famous Battle)=A Set of Common Clothes=A Belt Pouch Containing 2gp (Boros-minted 1-zino coins)</t>
@@ -388,13 +373,13 @@
     <t>A Uniform in the Style of your Unit=Indicative of your Rank=Horn with which to Summon Help=A Set of Manacles=A Pouch Containing 10 gp</t>
   </si>
   <si>
-    <t>A Set of Artisan’s Tools with which you are proficient=A Maker’s Mark Chisel used to mark your Handiwork with the Symbol of the Clan of Crafters you learned your Skill from=A Set of Traveler’s Clothes=A Pouch containing 5 gp=A Gem worth 10 gp</t>
+    <t>*Artisan’s Tools=A Maker’s Mark Chisel used to mark your Handiwork with the Symbol of the Clan of Crafters you learned your Skill from=A Set of Traveler’s Clothes=A Pouch containing 5 gp=A Gem worth 10 gp</t>
   </si>
   <si>
     <t>The Scholar’s Robes of your Cloister=A Writing Kit (Small Pouch with a Quill, Ink, Folded Parchment, and a Small Penknife)=A Borrowed Book on the Subject of your Current Study=A Pouch containing 10 gp</t>
   </si>
   <si>
-    <t>A Two-Person Tent=Artisan’s Tools=A Holy Symbol=A Set of Traveler’s Clothes=A Belt Pouch containing 5 gp</t>
+    <t>A Two-Person Tent=*Artisan’s Tools=A Holy Symbol=A Set of Traveler’s Clothes=A Belt Pouch containing 5 gp</t>
   </si>
   <si>
     <t>A Set of Fine Clothes=A Pouch containing 5 gp</t>
@@ -412,22 +397,22 @@
     <t>Fishing tackle=A Net=A Favorite Fishing Lure=A Set of Traveler’s Clothes=A Belt Pouch containing 10 gp</t>
   </si>
   <si>
-    <t>One Set of Artisan’s Tools=Merchant’s Scale=A Set of Fine Clothes=A Belt Pouch containing 10 gp</t>
-  </si>
-  <si>
-    <t>A disguise Kit=A Costume=A Pouch containing 10gp</t>
-  </si>
-  <si>
-    <t>One Musical Instrument=The Favor of an Admirer (Trinket)=A Costume=A Belt Pouch containing 15 gp.</t>
-  </si>
-  <si>
-    <t>One Set of Traveler’s Clothes=One Musical Instrument=Poorly Wrought Maps from your Homeland that Depict where you are in Faerûn=A Small Piece of Jewelry worth 10 gp in the Style of your Homeland’s Craftsmanship=A Pouch containing 5 gp</t>
-  </si>
-  <si>
-    <t>A Set of Artisan’s Tools=A Shovel=An Iron Pot=A Set of Common Clothes=A Pouch containing 10 gp</t>
-  </si>
-  <si>
-    <t>A Battered Alms Box=A Musical Instrument=A Cast-Off Military Jacket=A Set of Common Clothes=A Belt Pouch containing 10 gp</t>
+    <t>*Artisan’s Tools=Merchant’s Scale=A Set of Fine Clothes=A Belt Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Disguise Kit=A Costume=A Pouch containing 10gp</t>
+  </si>
+  <si>
+    <t>*Musical Instruments=The Favor of an Admirer (Trinket)=A Costume=A Belt Pouch containing 15 gp.</t>
+  </si>
+  <si>
+    <t>One Set of Traveler’s Clothes=*Musical Instruments=Poorly Wrought Maps from your Homeland that Depict where you are in Faerûn=A Small Piece of Jewelry worth 10 gp in the Style of your Homeland’s Craftsmanship=A Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>*Artisan’s Tools=A Shovel=An Iron Pot=A Set of Common Clothes=A Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A Battered Alms Box=*Musical Instruments=A Cast-Off Military Jacket=A Set of Common Clothes=A Belt Pouch containing 10 gp</t>
   </si>
   <si>
     <t>A Golgari Insignia=A Poisoner’s Kit=A Pet Beetle=A Set of Common Clothes=A Belt Pouch containing 10 gp worth of Mixed Coins</t>
@@ -436,16 +421,16 @@
     <t>A Gruul Insignia=A Hunting Trap=An Herbalism Kit=The Skull of a Boar=A Beast-Hide Cloak=A Set of Traveler’s Clothes=A Pouch containing 10gp (Azorius 1-zino coins)</t>
   </si>
   <si>
-    <t>One Gaming Set=A Lucky Charm=A Set of Fine Clothes=A Belt Pouch containing 15 gp</t>
+    <t>*Gaming Sets=A Lucky Charm=A Set of Fine Clothes=A Belt Pouch containing 15 gp</t>
   </si>
   <si>
     <t>A Mule=A Cart=A Letter of Introduction from your Guild=A Set of Traveler’s Clothes=A Belt Pouch containing 15 gp</t>
   </si>
   <si>
-    <t>A Set of Artisan’s Tools=A Letter of Introduction from your Guild=A Set of Traveler’s Clothes=A Belt Pouch containing 15 gp</t>
-  </si>
-  <si>
-    <t>Fishing tackle=Dice Set=A Set of Common Clothes=Rowboat=A Belt containing 5 gp</t>
+    <t>*Artisan’s Tools=A Letter of Introduction from your Guild=A Set of Traveler’s Clothes=A Belt Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>Fishing tackle=*Gaming Sets=A Set of Common Clothes=Rowboat=A Belt containing 5 gp</t>
   </si>
   <si>
     <t>Monster Hunter’s Pack=One Trinket of Special Significance</t>
@@ -463,10 +448,10 @@
     <t>A Set of Fine Clothes=House Signet Ring=Identification Papers=A Purse containing 20 gp</t>
   </si>
   <si>
-    <t>Your Inheritance=A Set of Traveler’s Clothes=A Musical Instrument=A Pouch containing 15 gp</t>
-  </si>
-  <si>
-    <t>A Simple Puzzle Box=A Scroll containing the Basic Teachings of the Five Gods=A Gaming Set=A Set of Common Clothes=A Pouch containing 15 gp</t>
+    <t>Your Inheritance=A Set of Traveler’s Clothes=*Musical Instruments=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>A Simple Puzzle Box=A Scroll containing the Basic Teachings of the Five Gods=*Gaming Sets=A Set of Common Clothes=A Pouch containing 15 gp</t>
   </si>
   <si>
     <t>A Holy Symbol=A Set of Traveler’s Clothes=A Pouch containing 15 gp</t>
@@ -475,7 +460,7 @@
     <t>A Set of Dark Common Clothes=Pack Saddle=Burglar’s Pack=A Pouch containing 5 gp</t>
   </si>
   <si>
-    <t>An Izzet Insignia=One Set of Artisan’s Tools=The Charred and Twisted remains of a Failed Experiment=A Hammer=A Block and Tackle=A Set of Common Clothes=A Belt Pouch containing 5 gp (Azorius 1-Zino Coins)</t>
+    <t>An Izzet Insignia=*Artisan’s Tools=The Charred and Twisted remains of a Failed Experiment=A Hammer=A Block and Tackle=A Set of Common Clothes=A Belt Pouch containing 5 gp (Azorius 1-Zino Coins)</t>
   </si>
   <si>
     <t>A Set of Fine Clothes=A Signet Ring=A Scroll of Pedigree=A Purse containing 25 gp</t>
@@ -1039,243 +1024,243 @@
         <v>80</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AF3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AI3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="AN3" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AP3" s="2" t="s">
         <v>80</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="R4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="AB4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="AP4" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="AQ4" s="2" t="s">
         <v>76</v>
@@ -1286,136 +1271,136 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AF5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AG5" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AH5" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AI5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AK5" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AL5" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AM5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AI5" s="2" t="s">
+      <c r="AN5" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AO5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AP5" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AQ5" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AM5" s="2" t="s">
+      <c r="AR5" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="AN5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AQ5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AR5" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before adding updated archetype code
</commit_message>
<xml_diff>
--- a/backgrounds/Attributes.xlsx
+++ b/backgrounds/Attributes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
   <si>
     <t>Acolyte</t>
   </si>
@@ -139,6 +139,39 @@
     <t>Knight</t>
   </si>
   <si>
+    <t>Mercenary Veteran</t>
+  </si>
+  <si>
+    <t>Mulmaster Aristocrat</t>
+  </si>
+  <si>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>Orzhov Representative</t>
+  </si>
+  <si>
+    <t>Outlander</t>
+  </si>
+  <si>
+    <t>Pirate</t>
+  </si>
+  <si>
+    <t>Phlan Insurgent</t>
+  </si>
+  <si>
+    <t>Phlan Refugee</t>
+  </si>
+  <si>
+    <t>Plaintiff</t>
+  </si>
+  <si>
+    <t>Rakdos Cultist</t>
+  </si>
+  <si>
+    <t>Rival Intern</t>
+  </si>
+  <si>
     <t>Smuggler</t>
   </si>
   <si>
@@ -238,6 +271,33 @@
     <t>History=Persuasion</t>
   </si>
   <si>
+    <t>Athletics=Persuasion</t>
+  </si>
+  <si>
+    <t>Deception=Performance</t>
+  </si>
+  <si>
+    <t>Intimidation=Religion</t>
+  </si>
+  <si>
+    <t>Survival=Athletics</t>
+  </si>
+  <si>
+    <t>Athletics=Perception</t>
+  </si>
+  <si>
+    <t>Stealth, Survival</t>
+  </si>
+  <si>
+    <t>Insight=Athletics</t>
+  </si>
+  <si>
+    <t>Medicine=Persuasion</t>
+  </si>
+  <si>
+    <t>History=Investigation</t>
+  </si>
+  <si>
     <t>Athletics=Deception</t>
   </si>
   <si>
@@ -310,6 +370,18 @@
     <t>Thieves’ Tools=*Artisan’s Tools</t>
   </si>
   <si>
+    <t>*Artisan’s tools=*Musical Instruments</t>
+  </si>
+  <si>
+    <t>Navigator’s Tools=Vehicles (Water)</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools=Vehicles (Land)</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools</t>
+  </si>
+  <si>
     <t>Any=Any</t>
   </si>
   <si>
@@ -464,6 +536,39 @@
   </si>
   <si>
     <t>A Set of Fine Clothes=A Signet Ring=A Scroll of Pedigree=A Purse containing 25 gp</t>
+  </si>
+  <si>
+    <t>A Uniform of your Company (Traveler’s Clothes in Quality)=An Insignia of your Rank=*Gaming Sets=A Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools=A Set of Fine Clothes=A Purse containing 10 gp</t>
+  </si>
+  <si>
+    <t>A set of Fine Clothes=A Signet Ring=A Scroll of Pedigree=A Purse containing 25 gp</t>
+  </si>
+  <si>
+    <t>An Orzhov Insignia=A Foot-Long Chain made of Ten Gold Coins=Vestments=A Set of Fine Clothes=A Pouch containing 1pp (an Orzhov-minted 10-Zino Coin)</t>
+  </si>
+  <si>
+    <t>A Staff=A Trophy from an Animal you killed=A Belt Pouch containing 10 gp=A Hunting Trap=A Set of Traveler’s Clothes.</t>
+  </si>
+  <si>
+    <t>A Belaying Pin (club)=50 feet of Silk Rope=A Lucky Charm=A Set of Common Clothes=A Belt Pouch containing 10 gp</t>
+  </si>
+  <si>
+    <t>A bag of 20 Caltrops=A Small Trinket that connects you to the Life you once had before the Occupation of Phlan=A Healer’s Kit=A Set of Dark Common Clothes that includes a Cloak and Hood=A Pouch containing 5 gp</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools=A Token of the Life you once knew=A Set of Traveler’s Clothes=A Pouch containing 15 gp</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools=Fine Clothes=20 gp</t>
+  </si>
+  <si>
+    <t>A Rakdos Insignia=*Musical Instruments=A Costume=A Hooded Lantern made of Wrought Iron=A 10-foot Length of Chain with Sharply Spiked Links=A tinderbox=10 torches=A Set of Common Clothes=A Belt Pouch containing 10 gp (A Mix of Azorius and Boros 1-zino coins)=A Bottle of Sweet, Red Juice</t>
+  </si>
+  <si>
+    <t>*Artisan’s tools=A Ledger from your Previous Employer containing a Small Piece of Useful Information=A Set of Fine Clothes=A Belt Pouch containing 10 gp</t>
   </si>
   <si>
     <t>A Fancy Leather Vest=A Set of Common Clothes=A Leather Pouch with 15 gp</t>
@@ -866,541 +971,706 @@
       <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="AS1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC2" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>84</v>
+        <v>119</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC3" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BA4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="AN5" s="2" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>152</v>
+        <v>176</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC5" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>